<commit_message>
Fixed failing test cases in Create Question Test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CreateQuestion.xlsx
+++ b/src/test/resources/testdata/CreateQuestion.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1106,11 +1107,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1457,13 +1458,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="19.625" customWidth="1"/>
     <col min="2" max="2" width="59.8125" customWidth="1"/>
@@ -1483,49 +1484,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1558,21 +1559,21 @@
         <v>3</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1605,21 +1606,21 @@
         <v>2</v>
       </c>
       <c r="J3">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="K3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1652,21 +1653,21 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="K4" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1699,21 +1700,21 @@
         <v>2</v>
       </c>
       <c r="J5">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="K5" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1746,726 +1747,21 @@
         <v>4</v>
       </c>
       <c r="J6">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="K6" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>12</v>
-      </c>
-      <c r="K7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>18</v>
-      </c>
-      <c r="K8" t="s">
-        <v>23</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10">
-        <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" t="s">
-        <v>90</v>
-      </c>
-      <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" t="s">
-        <v>96</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <v>20</v>
-      </c>
-      <c r="K12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H13" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13">
-        <v>25</v>
-      </c>
-      <c r="K13" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14">
-        <v>30</v>
-      </c>
-      <c r="K14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15" t="s">
-        <v>111</v>
-      </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15">
-        <v>20</v>
-      </c>
-      <c r="K15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
-      <c r="A16" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" t="s">
-        <v>117</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16">
-        <v>15</v>
-      </c>
-      <c r="K16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" t="s">
-        <v>120</v>
-      </c>
-      <c r="D17" t="s">
-        <v>121</v>
-      </c>
-      <c r="E17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F17" t="s">
-        <v>123</v>
-      </c>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>44</v>
-      </c>
-      <c r="I17" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>18</v>
-      </c>
-      <c r="K17" t="s">
-        <v>36</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" t="s">
-        <v>124</v>
-      </c>
-      <c r="B18" t="s">
-        <v>125</v>
-      </c>
-      <c r="C18" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" t="s">
-        <v>127</v>
-      </c>
-      <c r="E18" t="s">
-        <v>128</v>
-      </c>
-      <c r="F18" t="s">
-        <v>129</v>
-      </c>
-      <c r="G18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>22</v>
-      </c>
-      <c r="K18" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" t="s">
-        <v>133</v>
-      </c>
-      <c r="F19" t="s">
-        <v>134</v>
-      </c>
-      <c r="G19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" t="s">
-        <v>44</v>
-      </c>
-      <c r="I19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <v>25</v>
-      </c>
-      <c r="K19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" t="s">
-        <v>136</v>
-      </c>
-      <c r="C20" t="s">
-        <v>137</v>
-      </c>
-      <c r="D20" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G20" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <v>30</v>
-      </c>
-      <c r="K20" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" t="s">
-        <v>143</v>
-      </c>
-      <c r="D21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" t="s">
-        <v>145</v>
-      </c>
-      <c r="F21" t="s">
-        <v>146</v>
-      </c>
-      <c r="G21" t="s">
-        <v>44</v>
-      </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-      <c r="I21" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>15</v>
-      </c>
-      <c r="K21" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O21" s="3" t="s">
+      <c r="O6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2473,4 +1769,726 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11">
+        <v>18</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>30</v>
+      </c>
+      <c r="K14" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>